<commit_message>
update new folder rincian an asset update
</commit_message>
<xml_diff>
--- a/New folder/label rincian.xlsx
+++ b/New folder/label rincian.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="400">
   <si>
     <t>EKB/AC/001</t>
   </si>
@@ -346,15 +346,9 @@
     <t>Jam Sticker Dinding</t>
   </si>
   <si>
-    <t>Kain Pel</t>
-  </si>
-  <si>
     <t>Kemoceng</t>
   </si>
   <si>
-    <t>Keran Air</t>
-  </si>
-  <si>
     <t>Keranjang Plastik</t>
   </si>
   <si>
@@ -871,9 +865,6 @@
     <t>KYB</t>
   </si>
   <si>
-    <t>KRA</t>
-  </si>
-  <si>
     <t>KTS</t>
   </si>
   <si>
@@ -1217,6 +1208,12 @@
   </si>
   <si>
     <t>Stock</t>
+  </si>
+  <si>
+    <t>Alat Pel Lantai</t>
+  </si>
+  <si>
+    <t>Koridor Lt 2</t>
   </si>
 </sst>
 </file>
@@ -1568,11 +1565,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K350"/>
+  <dimension ref="A1:K370"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E202" sqref="E202"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" customHeight="1"/>
@@ -1586,7 +1583,7 @@
     <col min="8" max="8" width="20.140625" style="4" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -1872,7 +1869,7 @@
         <v>60</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>52</v>
@@ -2422,7 +2419,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>85</v>
@@ -2431,7 +2428,7 @@
         <v>28</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>52</v>
@@ -2442,7 +2439,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>86</v>
@@ -2473,22 +2470,22 @@
         <v>40</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>87</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="18.75" customHeight="1">
@@ -2499,16 +2496,16 @@
         <v>87</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="18.75" customHeight="1">
@@ -2519,16 +2516,16 @@
         <v>87</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="18.75" customHeight="1">
@@ -2539,16 +2536,16 @@
         <v>87</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="18.75" customHeight="1">
@@ -2559,16 +2556,16 @@
         <v>87</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="18.75" customHeight="1">
@@ -2579,16 +2576,16 @@
         <v>87</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="18.75" customHeight="1">
@@ -2599,16 +2596,16 @@
         <v>87</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="18.75" customHeight="1">
@@ -2619,16 +2616,16 @@
         <v>87</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="18.75" customHeight="1">
@@ -2639,16 +2636,16 @@
         <v>87</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="18.75" customHeight="1">
@@ -2659,7 +2656,7 @@
         <v>87</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>35</v>
@@ -2676,7 +2673,7 @@
         <v>87</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>36</v>
@@ -2693,16 +2690,16 @@
         <v>87</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="18.75" customHeight="1">
@@ -2713,16 +2710,16 @@
         <v>87</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="18.75" customHeight="1">
@@ -2733,16 +2730,16 @@
         <v>87</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="18.75" customHeight="1">
@@ -2753,16 +2750,16 @@
         <v>87</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="18.75" customHeight="1">
@@ -2773,16 +2770,16 @@
         <v>87</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="18.75" customHeight="1">
@@ -2793,16 +2790,16 @@
         <v>87</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="18.75" customHeight="1">
@@ -2813,16 +2810,16 @@
         <v>87</v>
       </c>
       <c r="E58" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="H58" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="H58" s="4" t="s">
-        <v>356</v>
-      </c>
       <c r="J58" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="18.75" customHeight="1">
@@ -2833,7 +2830,7 @@
         <v>87</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>25</v>
@@ -2850,10 +2847,10 @@
         <v>87</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>52</v>
@@ -2867,10 +2864,10 @@
         <v>87</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>52</v>
@@ -2884,7 +2881,7 @@
         <v>87</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H62" s="4" t="s">
         <v>34</v>
@@ -2901,7 +2898,7 @@
         <v>87</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H63" s="4" t="s">
         <v>22</v>
@@ -2918,7 +2915,7 @@
         <v>87</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H64" s="4" t="s">
         <v>24</v>
@@ -2935,10 +2932,10 @@
         <v>87</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>52</v>
@@ -2952,7 +2949,7 @@
         <v>87</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H66" s="4" t="s">
         <v>29</v>
@@ -2969,7 +2966,7 @@
         <v>87</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H67" s="4" t="s">
         <v>28</v>
@@ -2986,7 +2983,7 @@
         <v>87</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H68" s="4" t="s">
         <v>33</v>
@@ -3003,7 +3000,7 @@
         <v>87</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H69" s="4" t="s">
         <v>33</v>
@@ -3020,10 +3017,10 @@
         <v>87</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>52</v>
@@ -3037,10 +3034,10 @@
         <v>87</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>52</v>
@@ -3062,16 +3059,16 @@
         <v>72</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>88</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>52</v>
@@ -3082,7 +3079,7 @@
         <v>73</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>89</v>
@@ -3091,7 +3088,7 @@
         <v>34</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>52</v>
@@ -3108,7 +3105,7 @@
         <v>35</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>52</v>
@@ -3125,7 +3122,7 @@
         <v>36</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>52</v>
@@ -3192,16 +3189,16 @@
         <v>80</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>90</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>77</v>
@@ -3215,7 +3212,7 @@
         <v>81</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>91</v>
@@ -3241,7 +3238,7 @@
         <v>35</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>52</v>
@@ -3258,7 +3255,7 @@
         <v>29</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="J84" s="1" t="s">
         <v>52</v>
@@ -3272,16 +3269,16 @@
         <v>91</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H85" s="4" t="s">
         <v>22</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>52</v>
@@ -3292,7 +3289,7 @@
         <v>85</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>92</v>
@@ -3315,13 +3312,13 @@
         <v>93</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H87" s="4" t="s">
         <v>35</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="J87" s="1" t="s">
         <v>52</v>
@@ -3335,13 +3332,13 @@
         <v>93</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H88" s="4" t="s">
         <v>35</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J88" s="1" t="s">
         <v>52</v>
@@ -3355,13 +3352,13 @@
         <v>93</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H89" s="4" t="s">
         <v>35</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="J89" s="1" t="s">
         <v>52</v>
@@ -3375,13 +3372,13 @@
         <v>93</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H90" s="4" t="s">
         <v>35</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="J90" s="1" t="s">
         <v>52</v>
@@ -3395,13 +3392,13 @@
         <v>93</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H91" s="4" t="s">
         <v>36</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="J91" s="1" t="s">
         <v>52</v>
@@ -3415,13 +3412,13 @@
         <v>93</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H92" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="J92" s="1" t="s">
         <v>52</v>
@@ -3435,13 +3432,13 @@
         <v>93</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H93" s="4" t="s">
         <v>22</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="J93" s="1" t="s">
         <v>52</v>
@@ -3455,13 +3452,13 @@
         <v>93</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H94" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="J94" s="1" t="s">
         <v>52</v>
@@ -3475,13 +3472,13 @@
         <v>93</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H95" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="J95" s="1" t="s">
         <v>52</v>
@@ -3495,13 +3492,13 @@
         <v>93</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H96" s="4" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>52</v>
@@ -3515,13 +3512,13 @@
         <v>93</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H97" s="4" t="s">
         <v>29</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="J97" s="1" t="s">
         <v>52</v>
@@ -3535,13 +3532,13 @@
         <v>93</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H98" s="4" t="s">
         <v>28</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>52</v>
@@ -3555,10 +3552,10 @@
         <v>93</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="J99" s="1" t="s">
         <v>52</v>
@@ -3572,10 +3569,10 @@
         <v>93</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="J100" s="1" t="s">
         <v>52</v>
@@ -3589,10 +3586,10 @@
         <v>93</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="J101" s="1" t="s">
         <v>52</v>
@@ -3606,10 +3603,10 @@
         <v>93</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="J102" s="1" t="s">
         <v>52</v>
@@ -3623,10 +3620,10 @@
         <v>93</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="J103" s="1" t="s">
         <v>52</v>
@@ -3640,13 +3637,13 @@
         <v>93</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H104" s="4" t="s">
         <v>22</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="105" spans="1:10" ht="18.75" customHeight="1">
@@ -3654,7 +3651,7 @@
         <v>104</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>94</v>
@@ -3663,7 +3660,7 @@
         <v>35</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="106" spans="1:10" ht="18.75" customHeight="1">
@@ -3677,7 +3674,7 @@
         <v>36</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="107" spans="1:10" ht="18.75" customHeight="1">
@@ -3691,7 +3688,7 @@
         <v>38</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="18.75" customHeight="1">
@@ -3702,10 +3699,10 @@
         <v>94</v>
       </c>
       <c r="H108" s="4" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="109" spans="1:10" ht="18.75" customHeight="1">
@@ -3719,7 +3716,7 @@
         <v>34</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="110" spans="1:10" ht="18.75" customHeight="1">
@@ -3730,10 +3727,10 @@
         <v>94</v>
       </c>
       <c r="H110" s="4" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="111" spans="1:10" ht="18.75" customHeight="1">
@@ -3747,7 +3744,7 @@
         <v>29</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="112" spans="1:10" ht="18.75" customHeight="1">
@@ -3761,7 +3758,7 @@
         <v>28</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="113" spans="1:10" ht="18.75" customHeight="1">
@@ -3769,7 +3766,7 @@
         <v>112</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>95</v>
@@ -3778,10 +3775,10 @@
         <v>35</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="114" spans="1:10" ht="18.75" customHeight="1">
@@ -3795,10 +3792,10 @@
         <v>35</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="18.75" customHeight="1">
@@ -3812,10 +3809,10 @@
         <v>35</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="116" spans="1:10" ht="18.75" customHeight="1">
@@ -3829,10 +3826,10 @@
         <v>36</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="18.75" customHeight="1">
@@ -3846,10 +3843,10 @@
         <v>34</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="18.75" customHeight="1">
@@ -3863,10 +3860,10 @@
         <v>29</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="119" spans="1:10" ht="18.75" customHeight="1">
@@ -3880,10 +3877,10 @@
         <v>29</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="120" spans="1:10" ht="18.75" customHeight="1">
@@ -3897,10 +3894,10 @@
         <v>28</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="121" spans="1:10" ht="18.75" customHeight="1">
@@ -3914,10 +3911,10 @@
         <v>28</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="J121" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="122" spans="1:10" ht="18.75" customHeight="1">
@@ -3931,10 +3928,10 @@
         <v>28</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="J122" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="123" spans="1:10" ht="18.75" customHeight="1">
@@ -3948,10 +3945,10 @@
         <v>28</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="124" spans="1:10" ht="18.75" customHeight="1">
@@ -3968,7 +3965,7 @@
         <v>35</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="125" spans="1:10" ht="18.75" customHeight="1">
@@ -3979,10 +3976,10 @@
         <v>96</v>
       </c>
       <c r="H125" s="4" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="J125" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="126" spans="1:10" ht="18.75" customHeight="1">
@@ -3990,7 +3987,7 @@
         <v>125</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D126" s="4" t="s">
         <v>97</v>
@@ -3999,7 +3996,7 @@
         <v>28</v>
       </c>
       <c r="J126" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="127" spans="1:10" ht="18.75" customHeight="1">
@@ -4038,7 +4035,7 @@
         <v>98</v>
       </c>
       <c r="H129" s="4" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="J129" s="1" t="s">
         <v>52</v>
@@ -4052,7 +4049,7 @@
         <v>98</v>
       </c>
       <c r="H130" s="4" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="J130" s="1" t="s">
         <v>52</v>
@@ -4066,7 +4063,7 @@
         <v>98</v>
       </c>
       <c r="H131" s="4" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="J131" s="1" t="s">
         <v>52</v>
@@ -4175,7 +4172,7 @@
         <v>138</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D139" s="4" t="s">
         <v>99</v>
@@ -4192,13 +4189,13 @@
         <v>139</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D140" s="4" t="s">
         <v>100</v>
       </c>
       <c r="H140" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="J140" s="1" t="s">
         <v>52</v>
@@ -4212,7 +4209,7 @@
         <v>100</v>
       </c>
       <c r="H141" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="J141" s="1" t="s">
         <v>52</v>
@@ -4226,7 +4223,7 @@
         <v>100</v>
       </c>
       <c r="H142" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="J142" s="1" t="s">
         <v>52</v>
@@ -4240,7 +4237,7 @@
         <v>100</v>
       </c>
       <c r="H143" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="J143" s="1" t="s">
         <v>52</v>
@@ -4254,7 +4251,7 @@
         <v>100</v>
       </c>
       <c r="H144" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="J144" s="1" t="s">
         <v>52</v>
@@ -4268,7 +4265,7 @@
         <v>100</v>
       </c>
       <c r="H145" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="J145" s="1" t="s">
         <v>52</v>
@@ -4282,7 +4279,7 @@
         <v>100</v>
       </c>
       <c r="H146" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="J146" s="1" t="s">
         <v>52</v>
@@ -4296,7 +4293,7 @@
         <v>100</v>
       </c>
       <c r="H147" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="J147" s="1" t="s">
         <v>52</v>
@@ -4310,7 +4307,7 @@
         <v>100</v>
       </c>
       <c r="H148" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="J148" s="1" t="s">
         <v>52</v>
@@ -4324,7 +4321,7 @@
         <v>100</v>
       </c>
       <c r="H149" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="J149" s="1" t="s">
         <v>52</v>
@@ -4335,10 +4332,10 @@
         <v>149</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H150" s="4" t="s">
         <v>35</v>
@@ -4352,7 +4349,7 @@
         <v>150</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H151" s="4" t="s">
         <v>36</v>
@@ -4366,7 +4363,7 @@
         <v>151</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H152" s="4" t="s">
         <v>30</v>
@@ -4380,7 +4377,7 @@
         <v>152</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H153" s="4" t="s">
         <v>26</v>
@@ -4394,7 +4391,7 @@
         <v>153</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H154" s="4" t="s">
         <v>22</v>
@@ -4408,7 +4405,7 @@
         <v>154</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H155" s="4" t="s">
         <v>24</v>
@@ -4422,7 +4419,7 @@
         <v>155</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H156" s="4" t="s">
         <v>34</v>
@@ -4436,7 +4433,7 @@
         <v>156</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H157" s="4" t="s">
         <v>29</v>
@@ -4450,7 +4447,7 @@
         <v>157</v>
       </c>
       <c r="D158" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H158" s="4" t="s">
         <v>28</v>
@@ -4464,7 +4461,7 @@
         <v>158</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H159" s="4" t="s">
         <v>37</v>
@@ -4478,7 +4475,7 @@
         <v>159</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H160" s="4" t="s">
         <v>40</v>
@@ -4492,7 +4489,7 @@
         <v>160</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H161" s="4" t="s">
         <v>32</v>
@@ -4506,7 +4503,7 @@
         <v>161</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D162" s="4" t="s">
         <v>101</v>
@@ -4515,7 +4512,7 @@
         <v>37</v>
       </c>
       <c r="J162" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="163" spans="1:10" ht="18.75" customHeight="1">
@@ -4529,7 +4526,7 @@
         <v>37</v>
       </c>
       <c r="J163" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="164" spans="1:10" ht="18.75" customHeight="1">
@@ -4543,7 +4540,7 @@
         <v>37</v>
       </c>
       <c r="J164" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="165" spans="1:10" ht="18.75" customHeight="1">
@@ -4557,7 +4554,7 @@
         <v>37</v>
       </c>
       <c r="J165" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="166" spans="1:10" ht="18.75" customHeight="1">
@@ -4571,7 +4568,7 @@
         <v>37</v>
       </c>
       <c r="J166" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="167" spans="1:10" ht="18.75" customHeight="1">
@@ -4585,7 +4582,7 @@
         <v>37</v>
       </c>
       <c r="J167" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="168" spans="1:10" ht="18.75" customHeight="1">
@@ -4599,7 +4596,7 @@
         <v>37</v>
       </c>
       <c r="J168" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="169" spans="1:10" ht="18.75" customHeight="1">
@@ -4613,7 +4610,7 @@
         <v>37</v>
       </c>
       <c r="J169" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="170" spans="1:10" ht="18.75" customHeight="1">
@@ -4627,7 +4624,7 @@
         <v>37</v>
       </c>
       <c r="J170" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="171" spans="1:10" ht="18.75" customHeight="1">
@@ -4635,7 +4632,7 @@
         <v>170</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D171" s="4" t="s">
         <v>102</v>
@@ -4644,7 +4641,7 @@
         <v>37</v>
       </c>
       <c r="J171" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="172" spans="1:10" ht="18.75" customHeight="1">
@@ -4658,7 +4655,7 @@
         <v>40</v>
       </c>
       <c r="J172" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="173" spans="1:10" ht="18.75" customHeight="1">
@@ -4672,7 +4669,7 @@
         <v>40</v>
       </c>
       <c r="J173" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="174" spans="1:10" ht="18.75" customHeight="1">
@@ -4686,7 +4683,7 @@
         <v>40</v>
       </c>
       <c r="J174" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="175" spans="1:10" ht="18.75" customHeight="1">
@@ -4700,7 +4697,7 @@
         <v>40</v>
       </c>
       <c r="J175" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="176" spans="1:10" ht="18.75" customHeight="1">
@@ -4714,7 +4711,7 @@
         <v>40</v>
       </c>
       <c r="J176" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="177" spans="1:10" ht="18.75" customHeight="1">
@@ -4728,7 +4725,7 @@
         <v>40</v>
       </c>
       <c r="J177" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="178" spans="1:10" ht="18.75" customHeight="1">
@@ -4736,7 +4733,7 @@
         <v>177</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D178" s="4" t="s">
         <v>103</v>
@@ -4745,7 +4742,7 @@
         <v>37</v>
       </c>
       <c r="J178" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="179" spans="1:10" ht="18.75" customHeight="1">
@@ -4759,7 +4756,7 @@
         <v>37</v>
       </c>
       <c r="J179" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="180" spans="1:10" ht="18.75" customHeight="1">
@@ -4767,7 +4764,7 @@
         <v>179</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D180" s="4" t="s">
         <v>104</v>
@@ -4776,10 +4773,10 @@
         <v>34</v>
       </c>
       <c r="I180" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="J180" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="181" spans="1:10" ht="18.75" customHeight="1">
@@ -4793,10 +4790,10 @@
         <v>28</v>
       </c>
       <c r="I181" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="J181" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="182" spans="1:10" ht="18.75" customHeight="1">
@@ -4810,10 +4807,10 @@
         <v>24</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="J182" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="183" spans="1:10" ht="18.75" customHeight="1">
@@ -4827,10 +4824,10 @@
         <v>35</v>
       </c>
       <c r="I183" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J183" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="184" spans="1:10" ht="18.75" customHeight="1">
@@ -4838,7 +4835,7 @@
         <v>183</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D184" s="4" t="s">
         <v>105</v>
@@ -4847,7 +4844,7 @@
         <v>28</v>
       </c>
       <c r="J184" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="185" spans="1:10" ht="18.75" customHeight="1">
@@ -4861,7 +4858,7 @@
         <v>28</v>
       </c>
       <c r="J185" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="186" spans="1:10" ht="18.75" customHeight="1">
@@ -4875,7 +4872,7 @@
         <v>29</v>
       </c>
       <c r="J186" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="187" spans="1:10" ht="18.75" customHeight="1">
@@ -4889,7 +4886,7 @@
         <v>29</v>
       </c>
       <c r="J187" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="188" spans="1:10" ht="18.75" customHeight="1">
@@ -4897,7 +4894,7 @@
         <v>187</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D188" s="4" t="s">
         <v>106</v>
@@ -4909,7 +4906,7 @@
         <v>77</v>
       </c>
       <c r="J188" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="189" spans="1:10" ht="18.75" customHeight="1">
@@ -4923,16 +4920,16 @@
         <v>107</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H189" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I189" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="J189" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="190" spans="1:10" ht="18.75" customHeight="1">
@@ -4943,16 +4940,16 @@
         <v>107</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H190" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="I190" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="J190" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="191" spans="1:10" ht="18.75" customHeight="1">
@@ -4963,16 +4960,16 @@
         <v>107</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H191" s="4" t="s">
         <v>35</v>
       </c>
       <c r="I191" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="J191" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="192" spans="1:10" ht="18.75" customHeight="1">
@@ -4983,16 +4980,16 @@
         <v>107</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H192" s="4" t="s">
         <v>36</v>
       </c>
       <c r="I192" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="J192" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="193" spans="1:10" ht="18.75" customHeight="1">
@@ -5003,16 +5000,16 @@
         <v>107</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H193" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="I193" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="J193" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="194" spans="1:10" ht="18.75" customHeight="1">
@@ -5023,16 +5020,16 @@
         <v>107</v>
       </c>
       <c r="E194" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="H194" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="I194" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="H194" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="I194" s="1" t="s">
-        <v>399</v>
-      </c>
       <c r="J194" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="195" spans="1:10" ht="18.75" customHeight="1">
@@ -5043,16 +5040,16 @@
         <v>107</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H195" s="4" t="s">
         <v>22</v>
       </c>
       <c r="I195" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="J195" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="196" spans="1:10" ht="18.75" customHeight="1">
@@ -5063,16 +5060,16 @@
         <v>107</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H196" s="4" t="s">
         <v>22</v>
       </c>
       <c r="I196" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="J196" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="197" spans="1:10" ht="18.75" customHeight="1">
@@ -5083,16 +5080,16 @@
         <v>107</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H197" s="4" t="s">
         <v>22</v>
       </c>
       <c r="I197" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="J197" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="198" spans="1:10" ht="18.75" customHeight="1">
@@ -5103,16 +5100,16 @@
         <v>107</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H198" s="4" t="s">
         <v>22</v>
       </c>
       <c r="I198" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="J198" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="199" spans="1:10" ht="18.75" customHeight="1">
@@ -5120,7 +5117,7 @@
         <v>198</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D199" s="4" t="s">
         <v>108</v>
@@ -5129,7 +5126,7 @@
         <v>35</v>
       </c>
       <c r="J199" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="200" spans="1:10" ht="18.75" customHeight="1">
@@ -5137,13 +5134,16 @@
         <v>199</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D200" s="4" t="s">
         <v>109</v>
       </c>
       <c r="H200" s="4" t="s">
         <v>25</v>
+      </c>
+      <c r="J200" s="1" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="201" spans="1:10" ht="18.75" customHeight="1">
@@ -5156,6 +5156,9 @@
       <c r="H201" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="J201" s="1" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="202" spans="1:10" ht="18.75" customHeight="1">
       <c r="A202" s="1">
@@ -5167,6 +5170,9 @@
       <c r="H202" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="J202" s="1" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="203" spans="1:10" ht="18.75" customHeight="1">
       <c r="A203" s="1">
@@ -5178,956 +5184,1296 @@
       <c r="H203" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="J203" s="1" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="204" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A204" s="1">
+        <v>203</v>
+      </c>
       <c r="C204" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D204" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="H204" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="J204" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A205" s="1">
+        <v>204</v>
+      </c>
+      <c r="D205" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="H205" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="J205" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A206" s="1">
+        <v>205</v>
+      </c>
+      <c r="D206" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="H206" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="J206" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A207" s="1">
+        <v>206</v>
+      </c>
+      <c r="D207" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="H207" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="J207" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A208" s="1">
+        <v>207</v>
+      </c>
+      <c r="D208" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="H208" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="J208" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A209" s="1">
+        <v>208</v>
+      </c>
+      <c r="D209" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="H209" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="J209" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A210" s="1">
+        <v>209</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D210" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="D204" s="4" t="s">
+      <c r="E210" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="H210" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I210" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J210" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A211" s="1">
+        <v>210</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D211" s="4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="205" spans="1:10" ht="18.75" customHeight="1">
-      <c r="C205" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D205" s="4" t="s">
+      <c r="H211" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J211" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A212" s="1">
+        <v>211</v>
+      </c>
+      <c r="D212" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H212" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J212" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A213" s="1">
+        <v>212</v>
+      </c>
+      <c r="C213" s="1" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="206" spans="1:10" ht="18.75" customHeight="1">
-      <c r="C206" s="1" t="s">
+      <c r="D213" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="H213" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="J213" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A214" s="1">
+        <v>213</v>
+      </c>
+      <c r="D214" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="H214" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="J214" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A215" s="1">
+        <v>214</v>
+      </c>
+      <c r="C215" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D206" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="207" spans="1:10" ht="18.75" customHeight="1">
-      <c r="C207" s="1" t="s">
+      <c r="D215" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H215" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J215" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A216" s="1">
+        <v>215</v>
+      </c>
+      <c r="D216" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H216" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J216" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A217" s="1">
+        <v>216</v>
+      </c>
+      <c r="D217" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H217" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J217" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A218" s="1">
+        <v>217</v>
+      </c>
+      <c r="D218" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H218" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J218" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A219" s="1">
+        <v>218</v>
+      </c>
+      <c r="D219" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H219" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J219" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A220" s="1">
+        <v>219</v>
+      </c>
+      <c r="D220" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H220" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="J220" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A221" s="1">
+        <v>220</v>
+      </c>
+      <c r="D221" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H221" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="J221" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A222" s="1">
+        <v>221</v>
+      </c>
+      <c r="D222" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H222" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="J222" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A223" s="1">
+        <v>222</v>
+      </c>
+      <c r="D223" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H223" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="J223" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A224" s="1">
+        <v>223</v>
+      </c>
+      <c r="D224" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H224" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="J224" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A225" s="1">
+        <v>224</v>
+      </c>
+      <c r="D225" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H225" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="J225" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A226" s="1">
+        <v>225</v>
+      </c>
+      <c r="D226" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H226" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J226" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A227" s="1">
+        <v>226</v>
+      </c>
+      <c r="D227" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H227" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J227" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A228" s="1">
+        <v>227</v>
+      </c>
+      <c r="D228" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H228" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="J228" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A229" s="1">
+        <v>228</v>
+      </c>
+      <c r="D229" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H229" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="J229" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C230" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D230" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C231" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D231" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C232" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D232" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C233" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="D207" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="208" spans="1:10" ht="18.75" customHeight="1">
-      <c r="C208" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D208" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="209" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C209" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D209" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="210" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C210" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D210" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="211" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C211" s="1" t="s">
+      <c r="D233" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C234" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="D211" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="212" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C212" s="1" t="s">
+      <c r="D234" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C235" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="D212" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="213" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C213" s="1" t="s">
+      <c r="D235" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C236" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D213" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="214" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C214" s="1" t="s">
+      <c r="D236" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C237" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D214" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="215" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C215" s="1" t="s">
+      <c r="D237" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C238" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D238" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C239" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="D215" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="216" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C216" s="1" t="s">
+      <c r="D239" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C240" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="D216" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="217" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C217" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D217" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="218" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C218" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D218" s="4" t="s">
+      <c r="D240" s="4" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="219" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C219" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D219" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="220" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C220" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="D220" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="221" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C221" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D221" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="222" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C222" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="D222" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="223" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C223" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D223" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="224" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C224" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D224" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="225" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C225" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D225" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="226" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C226" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D226" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="227" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C227" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="D227" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="228" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C228" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="D228" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="229" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C229" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="D229" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="230" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C230" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="D230" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="231" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C231" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="D231" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="232" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C232" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="D232" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="233" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C233" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="D233" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="234" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C234" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="D234" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="235" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C235" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="D235" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="236" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C236" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="D236" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="237" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C237" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="D237" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="238" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C238" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="D238" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="239" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C239" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="D239" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="240" spans="3:4" ht="18.75" customHeight="1">
-      <c r="C240" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D240" s="4" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="241" spans="3:4" ht="18.75" customHeight="1">
       <c r="C241" s="1" t="s">
-        <v>312</v>
+        <v>281</v>
       </c>
       <c r="D241" s="4" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
     </row>
     <row r="242" spans="3:4" ht="18.75" customHeight="1">
       <c r="C242" s="1" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="D242" s="4" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
     </row>
     <row r="243" spans="3:4" ht="18.75" customHeight="1">
       <c r="C243" s="1" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="D243" s="4" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
     </row>
     <row r="244" spans="3:4" ht="18.75" customHeight="1">
       <c r="C244" s="1" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="D244" s="4" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
     </row>
     <row r="245" spans="3:4" ht="18.75" customHeight="1">
       <c r="C245" s="1" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="D245" s="4" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
     </row>
     <row r="246" spans="3:4" ht="18.75" customHeight="1">
       <c r="C246" s="1" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
       <c r="D246" s="4" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
     </row>
     <row r="247" spans="3:4" ht="18.75" customHeight="1">
       <c r="C247" s="1" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="D247" s="4" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
     </row>
     <row r="248" spans="3:4" ht="18.75" customHeight="1">
       <c r="C248" s="1" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
       <c r="D248" s="4" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
     </row>
     <row r="249" spans="3:4" ht="18.75" customHeight="1">
       <c r="C249" s="1" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="D249" s="4" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
     </row>
     <row r="250" spans="3:4" ht="18.75" customHeight="1">
       <c r="C250" s="1" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="D250" s="4" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
     </row>
     <row r="251" spans="3:4" ht="18.75" customHeight="1">
       <c r="C251" s="1" t="s">
-        <v>321</v>
+        <v>300</v>
       </c>
       <c r="D251" s="4" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
     </row>
     <row r="252" spans="3:4" ht="18.75" customHeight="1">
       <c r="C252" s="1" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="D252" s="4" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
     </row>
     <row r="253" spans="3:4" ht="18.75" customHeight="1">
       <c r="C253" s="1" t="s">
-        <v>324</v>
+        <v>302</v>
       </c>
       <c r="D253" s="4" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
     </row>
     <row r="254" spans="3:4" ht="18.75" customHeight="1">
       <c r="C254" s="1" t="s">
-        <v>325</v>
+        <v>303</v>
       </c>
       <c r="D254" s="4" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
     </row>
     <row r="255" spans="3:4" ht="18.75" customHeight="1">
       <c r="C255" s="1" t="s">
-        <v>326</v>
+        <v>304</v>
       </c>
       <c r="D255" s="4" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
     </row>
     <row r="256" spans="3:4" ht="18.75" customHeight="1">
       <c r="C256" s="1" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="D256" s="4" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
     </row>
     <row r="257" spans="3:4" ht="18.75" customHeight="1">
       <c r="C257" s="1" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="D257" s="4" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
     </row>
     <row r="258" spans="3:4" ht="18.75" customHeight="1">
       <c r="C258" s="1" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="D258" s="4" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
     </row>
     <row r="259" spans="3:4" ht="18.75" customHeight="1">
       <c r="C259" s="1" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="D259" s="4" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
     </row>
     <row r="260" spans="3:4" ht="18.75" customHeight="1">
       <c r="C260" s="1" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="D260" s="4" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
     </row>
     <row r="261" spans="3:4" ht="18.75" customHeight="1">
       <c r="C261" s="1" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="D261" s="4" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
     </row>
     <row r="262" spans="3:4" ht="18.75" customHeight="1">
       <c r="C262" s="1" t="s">
-        <v>331</v>
+        <v>310</v>
       </c>
       <c r="D262" s="4" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
     </row>
     <row r="263" spans="3:4" ht="18.75" customHeight="1">
       <c r="C263" s="1" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="D263" s="4" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
     </row>
     <row r="264" spans="3:4" ht="18.75" customHeight="1">
       <c r="C264" s="1" t="s">
-        <v>333</v>
+        <v>300</v>
       </c>
       <c r="D264" s="4" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
     </row>
     <row r="265" spans="3:4" ht="18.75" customHeight="1">
       <c r="C265" s="1" t="s">
-        <v>334</v>
+        <v>311</v>
       </c>
       <c r="D265" s="4" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
     </row>
     <row r="266" spans="3:4" ht="18.75" customHeight="1">
       <c r="C266" s="1" t="s">
-        <v>335</v>
+        <v>312</v>
       </c>
       <c r="D266" s="4" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
     </row>
     <row r="267" spans="3:4" ht="18.75" customHeight="1">
       <c r="C267" s="1" t="s">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="D267" s="4" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
     </row>
     <row r="268" spans="3:4" ht="18.75" customHeight="1">
       <c r="C268" s="1" t="s">
-        <v>337</v>
+        <v>314</v>
       </c>
       <c r="D268" s="4" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
     </row>
     <row r="269" spans="3:4" ht="18.75" customHeight="1">
       <c r="C269" s="1" t="s">
-        <v>338</v>
+        <v>315</v>
       </c>
       <c r="D269" s="4" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
     </row>
     <row r="270" spans="3:4" ht="18.75" customHeight="1">
       <c r="C270" s="1" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="D270" s="4" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
     </row>
     <row r="271" spans="3:4" ht="18.75" customHeight="1">
       <c r="C271" s="1" t="s">
-        <v>340</v>
+        <v>318</v>
       </c>
       <c r="D271" s="4" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
     </row>
     <row r="272" spans="3:4" ht="18.75" customHeight="1">
       <c r="C272" s="1" t="s">
-        <v>341</v>
+        <v>320</v>
       </c>
       <c r="D272" s="4" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
     </row>
     <row r="273" spans="3:4" ht="18.75" customHeight="1">
       <c r="C273" s="1" t="s">
-        <v>342</v>
+        <v>321</v>
       </c>
       <c r="D273" s="4" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
     </row>
     <row r="274" spans="3:4" ht="18.75" customHeight="1">
       <c r="C274" s="1" t="s">
-        <v>343</v>
+        <v>322</v>
       </c>
       <c r="D274" s="4" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
     </row>
     <row r="275" spans="3:4" ht="18.75" customHeight="1">
       <c r="C275" s="1" t="s">
-        <v>344</v>
+        <v>323</v>
       </c>
       <c r="D275" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="276" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C276" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D276" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="277" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C277" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D277" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="278" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C278" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D278" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="279" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C279" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D279" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="280" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C280" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D280" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="281" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C281" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D281" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="282" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C282" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D282" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="283" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C283" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D283" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="284" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C284" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D284" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="285" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C285" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D285" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="286" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C286" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D286" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="287" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C287" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D287" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="288" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C288" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D288" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="289" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C289" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D289" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="290" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C290" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D290" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="291" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C291" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D291" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="292" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C292" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D292" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="293" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C293" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D293" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="294" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C294" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D294" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="295" spans="3:4" ht="18.75" customHeight="1">
+      <c r="C295" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D295" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="296" spans="3:4" ht="18.75" customHeight="1">
+      <c r="D296" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="297" spans="3:4" ht="18.75" customHeight="1">
+      <c r="D297" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="276" spans="3:4" ht="18.75" customHeight="1">
-      <c r="D276" s="4" t="s">
+    <row r="298" spans="3:4" ht="18.75" customHeight="1">
+      <c r="D298" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="277" spans="3:4" ht="18.75" customHeight="1">
-      <c r="D277" s="4" t="s">
+    <row r="299" spans="3:4" ht="18.75" customHeight="1">
+      <c r="D299" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="278" spans="3:4" ht="18.75" customHeight="1">
-      <c r="D278" s="4" t="s">
+    <row r="300" spans="3:4" ht="18.75" customHeight="1">
+      <c r="D300" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="279" spans="3:4" ht="18.75" customHeight="1">
-      <c r="D279" s="4" t="s">
+    <row r="301" spans="3:4" ht="18.75" customHeight="1">
+      <c r="D301" s="4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="280" spans="3:4" ht="18.75" customHeight="1">
-      <c r="D280" s="4" t="s">
+    <row r="302" spans="3:4" ht="18.75" customHeight="1">
+      <c r="D302" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="281" spans="3:4" ht="18.75" customHeight="1">
-      <c r="D281" s="4" t="s">
+    <row r="303" spans="3:4" ht="18.75" customHeight="1">
+      <c r="D303" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="282" spans="3:4" ht="18.75" customHeight="1">
-      <c r="D282" s="4" t="s">
+    <row r="304" spans="3:4" ht="18.75" customHeight="1">
+      <c r="D304" s="4" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="283" spans="3:4" ht="18.75" customHeight="1">
-      <c r="D283" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="284" spans="3:4" ht="18.75" customHeight="1">
-      <c r="D284" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="285" spans="3:4" ht="18.75" customHeight="1">
-      <c r="D285" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="286" spans="3:4" ht="18.75" customHeight="1">
-      <c r="D286" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="287" spans="3:4" ht="18.75" customHeight="1">
-      <c r="D287" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="288" spans="3:4" ht="18.75" customHeight="1">
-      <c r="D288" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="289" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D289" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="290" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D290" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="291" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D291" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="292" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D292" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="293" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D293" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="294" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D294" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="295" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D295" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="296" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D296" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="297" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D297" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="298" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D298" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="299" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D299" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="300" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D300" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="301" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D301" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="302" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D302" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="303" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D303" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="304" spans="4:4" ht="18.75" customHeight="1">
-      <c r="D304" s="4" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="305" spans="4:4" ht="18.75" customHeight="1">
       <c r="D305" s="4" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
     </row>
     <row r="306" spans="4:4" ht="18.75" customHeight="1">
       <c r="D306" s="4" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
     </row>
     <row r="307" spans="4:4" ht="18.75" customHeight="1">
       <c r="D307" s="4" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
     </row>
     <row r="308" spans="4:4" ht="18.75" customHeight="1">
       <c r="D308" s="4" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
     </row>
     <row r="309" spans="4:4" ht="18.75" customHeight="1">
       <c r="D309" s="4" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
     </row>
     <row r="310" spans="4:4" ht="18.75" customHeight="1">
       <c r="D310" s="4" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="311" spans="4:4" ht="18.75" customHeight="1">
       <c r="D311" s="4" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
     </row>
     <row r="312" spans="4:4" ht="18.75" customHeight="1">
       <c r="D312" s="4" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
     </row>
     <row r="313" spans="4:4" ht="18.75" customHeight="1">
       <c r="D313" s="4" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
     </row>
     <row r="314" spans="4:4" ht="18.75" customHeight="1">
       <c r="D314" s="4" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
     </row>
     <row r="315" spans="4:4" ht="18.75" customHeight="1">
       <c r="D315" s="4" t="s">
-        <v>220</v>
+        <v>198</v>
       </c>
     </row>
     <row r="316" spans="4:4" ht="18.75" customHeight="1">
       <c r="D316" s="4" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
     </row>
     <row r="317" spans="4:4" ht="18.75" customHeight="1">
       <c r="D317" s="4" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
     </row>
     <row r="318" spans="4:4" ht="18.75" customHeight="1">
       <c r="D318" s="4" t="s">
-        <v>223</v>
+        <v>201</v>
       </c>
     </row>
     <row r="319" spans="4:4" ht="18.75" customHeight="1">
       <c r="D319" s="4" t="s">
-        <v>224</v>
+        <v>202</v>
       </c>
     </row>
     <row r="320" spans="4:4" ht="18.75" customHeight="1">
       <c r="D320" s="4" t="s">
-        <v>225</v>
+        <v>203</v>
       </c>
     </row>
     <row r="321" spans="4:4" ht="18.75" customHeight="1">
       <c r="D321" s="4" t="s">
-        <v>226</v>
+        <v>204</v>
       </c>
     </row>
     <row r="322" spans="4:4" ht="18.75" customHeight="1">
       <c r="D322" s="4" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
     </row>
     <row r="323" spans="4:4" ht="18.75" customHeight="1">
       <c r="D323" s="4" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
     </row>
     <row r="324" spans="4:4" ht="18.75" customHeight="1">
       <c r="D324" s="4" t="s">
-        <v>229</v>
+        <v>207</v>
       </c>
     </row>
     <row r="325" spans="4:4" ht="18.75" customHeight="1">
       <c r="D325" s="4" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
     </row>
     <row r="326" spans="4:4" ht="18.75" customHeight="1">
       <c r="D326" s="4" t="s">
-        <v>231</v>
+        <v>209</v>
       </c>
     </row>
     <row r="327" spans="4:4" ht="18.75" customHeight="1">
       <c r="D327" s="4" t="s">
-        <v>232</v>
+        <v>210</v>
       </c>
     </row>
     <row r="328" spans="4:4" ht="18.75" customHeight="1">
       <c r="D328" s="4" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
     </row>
     <row r="329" spans="4:4" ht="18.75" customHeight="1">
       <c r="D329" s="4" t="s">
-        <v>234</v>
+        <v>212</v>
       </c>
     </row>
     <row r="330" spans="4:4" ht="18.75" customHeight="1">
       <c r="D330" s="4" t="s">
-        <v>235</v>
+        <v>213</v>
       </c>
     </row>
     <row r="331" spans="4:4" ht="18.75" customHeight="1">
       <c r="D331" s="4" t="s">
-        <v>236</v>
+        <v>214</v>
       </c>
     </row>
     <row r="332" spans="4:4" ht="18.75" customHeight="1">
       <c r="D332" s="4" t="s">
-        <v>237</v>
+        <v>215</v>
       </c>
     </row>
     <row r="333" spans="4:4" ht="18.75" customHeight="1">
       <c r="D333" s="4" t="s">
-        <v>238</v>
+        <v>216</v>
       </c>
     </row>
     <row r="334" spans="4:4" ht="18.75" customHeight="1">
       <c r="D334" s="4" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
     </row>
     <row r="335" spans="4:4" ht="18.75" customHeight="1">
       <c r="D335" s="4" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
     </row>
     <row r="336" spans="4:4" ht="18.75" customHeight="1">
       <c r="D336" s="4" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
     </row>
     <row r="337" spans="4:4" ht="18.75" customHeight="1">
       <c r="D337" s="4" t="s">
-        <v>242</v>
+        <v>220</v>
       </c>
     </row>
     <row r="338" spans="4:4" ht="18.75" customHeight="1">
       <c r="D338" s="4" t="s">
-        <v>243</v>
+        <v>221</v>
       </c>
     </row>
     <row r="339" spans="4:4" ht="18.75" customHeight="1">
       <c r="D339" s="4" t="s">
-        <v>244</v>
+        <v>222</v>
       </c>
     </row>
     <row r="340" spans="4:4" ht="18.75" customHeight="1">
       <c r="D340" s="4" t="s">
-        <v>245</v>
+        <v>223</v>
       </c>
     </row>
     <row r="341" spans="4:4" ht="18.75" customHeight="1">
       <c r="D341" s="4" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
     </row>
     <row r="342" spans="4:4" ht="18.75" customHeight="1">
       <c r="D342" s="4" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
     </row>
     <row r="343" spans="4:4" ht="18.75" customHeight="1">
       <c r="D343" s="4" t="s">
-        <v>248</v>
+        <v>226</v>
       </c>
     </row>
     <row r="344" spans="4:4" ht="18.75" customHeight="1">
       <c r="D344" s="4" t="s">
-        <v>249</v>
+        <v>227</v>
       </c>
     </row>
     <row r="345" spans="4:4" ht="18.75" customHeight="1">
       <c r="D345" s="4" t="s">
-        <v>250</v>
+        <v>228</v>
       </c>
     </row>
     <row r="346" spans="4:4" ht="18.75" customHeight="1">
       <c r="D346" s="4" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
     </row>
     <row r="347" spans="4:4" ht="18.75" customHeight="1">
       <c r="D347" s="4" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
     </row>
     <row r="348" spans="4:4" ht="18.75" customHeight="1">
       <c r="D348" s="4" t="s">
-        <v>253</v>
+        <v>231</v>
       </c>
     </row>
     <row r="349" spans="4:4" ht="18.75" customHeight="1">
       <c r="D349" s="4" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
     </row>
     <row r="350" spans="4:4" ht="18.75" customHeight="1">
       <c r="D350" s="4" t="s">
-        <v>255</v>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="351" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D351" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="352" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D352" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="353" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D353" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="354" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D354" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="355" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D355" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="356" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D356" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="357" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D357" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="358" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D358" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="359" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D359" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="360" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D360" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="361" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D361" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="362" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D362" s="4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="363" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D363" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="364" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D364" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="365" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D365" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="366" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D366" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="367" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D367" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="368" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D368" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="369" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D369" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="370" spans="4:4" ht="18.75" customHeight="1">
+      <c r="D370" s="4" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>